<commit_message>
Fix 3.2 beta3 (#572)
* beta3

* better code

* /app/redirect

* topnav

* feat: topnav

* fix: 表单公式字段相互使用死循环

* better: TopNav

* fix: Decimal wrapValue on new

* feat: excel模板图片仅支持导出第一张

* fix: getStorageFile

---------

Co-authored-by: devezhao <zhaofang123@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/report-template-v3.xlsx
+++ b/src/test/resources/report-template-v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\rebuild\rebuild\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEB7E3D-A1AA-4BB3-9B97-7E3833AFEEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41657190-EE31-4B55-96D8-152E350CE046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>条码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>你好 {BARCODE}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -48,6 +44,18 @@
   </si>
   <si>
     <t xml:space="preserve">  {modifiedOn}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BARCODE}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{IMAGE}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -392,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -405,26 +413,32 @@
     <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>